<commit_message>
fix issue with mapping
</commit_message>
<xml_diff>
--- a/Examples/Sample.xlsx
+++ b/Examples/Sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\all-in-one-chatbot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\all-in-one-chatbot\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B122AE-911E-4D1E-97AA-FF498D2340A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4705D5-4C55-4BB7-B308-370E027F28BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="3885" windowWidth="21600" windowHeight="11295" xr2:uid="{E299C785-3DD1-4D5B-9742-136C5A5DCA19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E299C785-3DD1-4D5B-9742-136C5A5DCA19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Question</t>
   </si>
@@ -59,21 +59,12 @@
     <t>use_app_gw</t>
   </si>
   <si>
-    <t>Azure Application Gateway is a web traffic load balancer that enables you to manage traffic to your web application. It operates at the application layer (OSI layer 7) and routes traffic based on the content of the request, such as the URL or HTTP header. It features a web application firewall and intelligent layer 7 routing.</t>
-  </si>
-  <si>
     <t>What is OSI?</t>
   </si>
   <si>
-    <t>The Open Systems Interconnection (OSI) model is a conceptual framework that explains how data is transmitted between computers. It was developed by the International Organization for Standardization (ISO) in 1984. The OSI model provides a theoretical foundation for understanding network communication, although it is not directly implemented in its entirety in real-world networking hardware or software</t>
-  </si>
-  <si>
     <t>Does it support private connection to the backend? Just say Yes or No.</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>use_waf</t>
   </si>
   <si>
@@ -87,6 +78,27 @@
   </si>
   <si>
     <t>Azure Firewall is a cloud-native and intelligent network firewall security service that provides the best of breed threat protection for your cloud workloads running in Azure. It's a fully stateful firewall as a service with built-in high availability and unrestricted cloud scalability. It provides both east-west and north-south traffic inspection. [doc0]</t>
+  </si>
+  <si>
+    <t>out_of_domain</t>
+  </si>
+  <si>
+    <t>Tell me a joke about Firewall</t>
+  </si>
+  <si>
+    <t>Sorry, I am a chat bot that can answer questions on Azure.</t>
+  </si>
+  <si>
+    <t>OUT_OF_DOMAIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azure Application Gateway is a web traffic load balancer that enables you to manage traffic to your web application. It operates at the application layer (OSI layer 7) and routes traffic based on the content of the request, such as the URL or HTTP header. It features a web application firewall and intelligent layer 7 routing. [doc0] </t>
+  </si>
+  <si>
+    <t>Yes [doc0]</t>
+  </si>
+  <si>
+    <t>[doo0],Application Gateway Private Link,https://learn.microsoft.com/en-us/azure/application-gateway/private-link</t>
   </si>
 </sst>
 </file>
@@ -458,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6773FF-2ECA-43DC-AD8F-B13B2762B17D}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +498,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -497,10 +509,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -508,13 +523,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -522,30 +537,47 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
       <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>